<commit_message>
env's consolidated. (was confused by when saving the .env, 3/3 batchdata keys with all permissions/scopes of v1 batch that made the call work were there, however one change not observed was DEVELOPERNAME= there was no space between = and G in the editted version and when i rewrote over it, there was so hopefilly just that was changed And not anything else in terms of the API keys. But we did get successful API calls for batch data complete now that templating is just the raw template with the input master, output master, and the other sheets (namely, config, blacklist names) which we should plug back into the logic of the scripts. But we'll hold off on that as we are preparing to introduce CRM template or excuse me, v300 dialer template and the v300 dialer aspect. Then we'll go back and fix all the batch data stuff.
</commit_message>
<xml_diff>
--- a/Batchdata/tests/batchdata_local_input.xlsx
+++ b/Batchdata/tests/batchdata_local_input.xlsx
@@ -744,7 +744,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://api.batchdata.io</t>
+          <t>https://api.batchdata.com/api/v1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -983,10 +983,8 @@
           <t>JPBD ONE, LLC</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>23801257</t>
-        </is>
+      <c r="D2" t="n">
+        <v>23801257</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1013,7 +1011,6 @@
           <t>PO BOX 624</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>80814</t>
@@ -1024,17 +1021,11 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
           <t>Maricopa</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
           <t>Derived from eCorp search: JPBD ONE LLC</t>
@@ -1057,10 +1048,8 @@
           <t>JPBD ONE, LLC</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>23801257</t>
-        </is>
+      <c r="D3" t="n">
+        <v>23801257</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1087,7 +1076,6 @@
           <t>4531 E. Beryl Lane</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
           <t>85028</t>
@@ -1098,17 +1086,11 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
           <t>Maricopa</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr">
         <is>
           <t>Derived from eCorp search: JPBD ONE LLC</t>
@@ -1131,10 +1113,8 @@
           <t>ZION PROPERTY PARTNERS LLC</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>23800981</t>
-        </is>
+      <c r="D4" t="n">
+        <v>23800981</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -1161,7 +1141,6 @@
           <t>4539 N 22ND STREET STE R</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
           <t>AZ 85016</t>
@@ -1172,17 +1151,11 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
           <t>Maricopa</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr">
         <is>
           <t>Derived from eCorp search: ZION PROPERTY LLC</t>
@@ -1205,10 +1178,8 @@
           <t>Leric Enterprises, LLC</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>23774701</t>
-        </is>
+      <c r="D5" t="n">
+        <v>23774701</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1235,7 +1206,6 @@
           <t>1933 w holden dr</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
           <t>85085</t>
@@ -1246,17 +1216,11 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
           <t>Maricopa</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr">
         <is>
           <t>Derived from eCorp search: LERIC ENTERPRISES LLC</t>
@@ -1578,7 +1542,6 @@
           <t>mailing_city</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1591,7 +1554,6 @@
           <t>mailing_state</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1757,7 +1719,6 @@
           <t>unit_type/unit_number</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1770,7 +1731,6 @@
           <t>city/state/zip/zip4</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">

</xml_diff>